<commit_message>
Update to new version of Ampersand compiler
</commit_message>
<xml_diff>
--- a/ProjectAdministration.xlsx
+++ b/ProjectAdministration.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Git\Project-administration\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="18195" windowHeight="11760"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="18195" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Projects" sheetId="1" r:id="rId1"/>
-    <sheet name="People" sheetId="2" r:id="rId2"/>
+    <sheet name="#Projects" sheetId="1" r:id="rId1"/>
+    <sheet name="#People" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="92">
   <si>
     <t>Project</t>
   </si>
@@ -185,21 +190,6 @@
     <t>Succes</t>
   </si>
   <si>
-    <t>[Person,]</t>
-  </si>
-  <si>
-    <t>p10001,p10002,p10003</t>
-  </si>
-  <si>
-    <t>p10001,p10003,p10004,p10005</t>
-  </si>
-  <si>
-    <t>p10002,p10003,p10005</t>
-  </si>
-  <si>
-    <t>p10006,p10009,p10010</t>
-  </si>
-  <si>
     <t>Completed</t>
   </si>
   <si>
@@ -303,12 +293,15 @@
   </si>
   <si>
     <t>1970_13</t>
+  </si>
+  <si>
+    <t>[Members]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -380,6 +373,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -427,7 +423,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -460,9 +456,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -495,6 +508,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -670,11 +700,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,10 +716,9 @@
     <col min="5" max="5" width="16.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="8" width="47.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -706,16 +735,13 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -737,19 +763,16 @@
       <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
         <v>49</v>
@@ -764,19 +787,16 @@
       <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="H3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>50</v>
@@ -791,13 +811,10 @@
       <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>18</v>
@@ -811,13 +828,10 @@
       <c r="G5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>6</v>
@@ -830,9 +844,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>20</v>
@@ -849,9 +863,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>22</v>
@@ -872,14 +886,134 @@
       <c r="G8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="3"/>
       <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -888,11 +1022,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,10 +1043,10 @@
         <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>29</v>
@@ -927,10 +1061,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>47</v>
@@ -945,10 +1079,10 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
         <v>30</v>
@@ -963,10 +1097,10 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>33</v>
@@ -978,10 +1112,10 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>34</v>
@@ -993,10 +1127,10 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
         <v>30</v>
@@ -1011,10 +1145,10 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>36</v>
@@ -1026,10 +1160,10 @@
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>37</v>
@@ -1041,10 +1175,10 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>38</v>
@@ -1056,10 +1190,10 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>39</v>
@@ -1071,10 +1205,10 @@
         <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>40</v>
@@ -1086,10 +1220,10 @@
         <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>41</v>
@@ -1101,10 +1235,10 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>42</v>
@@ -1116,10 +1250,10 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>31</v>
@@ -1128,18 +1262,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E14" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="E6" r:id="rId5"/>
-    <hyperlink ref="E7" r:id="rId6"/>
-    <hyperlink ref="E8" r:id="rId7"/>
-    <hyperlink ref="E9" r:id="rId8"/>
-    <hyperlink ref="E10" r:id="rId9"/>
-    <hyperlink ref="E11" r:id="rId10"/>
-    <hyperlink ref="E12" r:id="rId11"/>
-    <hyperlink ref="E13" r:id="rId12"/>
+    <hyperlink ref="E14" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="E12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Upgrade to new Ampersand 4.0 CLI and simplify docker and docker-compose script
</commit_message>
<xml_diff>
--- a/ProjectAdministration.xlsx
+++ b/ProjectAdministration.xlsx
@@ -1,21 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Git\Project-administration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\project-administration\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BB983B-A216-45CE-BC53-D56985C62715}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="18195" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32310" yWindow="3510" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Projects" sheetId="1" r:id="rId1"/>
     <sheet name="#People" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1026,7 +1035,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>